<commit_message>
Fixed test build. Refactored DocumentContent to interface only.
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Linked Data From CSV" sheetId="1" r:id="rId1"/>
-    <sheet name="New Pivot" sheetId="4" r:id="rId2"/>
-    <sheet name="Pivot" sheetId="3" r:id="rId3"/>
+    <sheet name="Pivot" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$45</definedName>
+    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$46</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
   <si>
     <t>mlclient::internals::AuthenticatingProxy::putSync</t>
   </si>
@@ -139,13 +138,16 @@
   </si>
   <si>
     <t>ConnectionSearchTest::testQueryText</t>
+  </si>
+  <si>
+    <t>ConnectionSearchTest::testWordQuery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +170,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,8 +204,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -196,12 +216,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -210,13 +232,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42501.309907986113" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="44">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42502.295535185185" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="45">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:B45" sheet="Linked Data From CSV"/>
+    <worksheetSource ref="A1:B46" sheet="Linked Data From CSV"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Function name" numFmtId="0">
-      <sharedItems count="21">
+      <sharedItems count="22">
         <s v="mlclient::internals::AuthenticatingProxy::putSync"/>
         <s v="mlclient::Connection::saveDocument"/>
         <s v="ConnectionDocumentCrudTest::testSaveJson"/>
@@ -238,10 +260,11 @@
         <s v="mlclient::Connection::search"/>
         <s v="ConnectionSearchTest::testEmptySearch"/>
         <s v="ConnectionSearchTest::testQueryText"/>
+        <s v="ConnectionSearchTest::testWordQuery"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="29"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="31"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -253,14 +276,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="44">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="45">
   <r>
     <x v="0"/>
-    <n v="22"/>
+    <n v="21"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="22"/>
+    <n v="21"/>
   </r>
   <r>
     <x v="2"/>
@@ -272,19 +295,19 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="4"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="4"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="6"/>
-    <n v="4"/>
+    <n v="6"/>
   </r>
   <r>
     <x v="7"/>
-    <n v="4"/>
+    <n v="3"/>
   </r>
   <r>
     <x v="8"/>
@@ -312,15 +335,55 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="3"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="3"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="11"/>
-    <n v="4"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="6"/>
   </r>
   <r>
     <x v="7"/>
@@ -331,48 +394,28 @@
     <n v="3"/>
   </r>
   <r>
-    <x v="12"/>
+    <x v="15"/>
     <n v="3"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <n v="5"/>
+    <x v="16"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="3"/>
     <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <n v="3"/>
+    <x v="17"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="31"/>
   </r>
   <r>
     <x v="16"/>
@@ -384,15 +427,15 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="28"/>
+    <n v="19"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="28"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <n v="29"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="20"/>
   </r>
   <r>
     <x v="16"/>
@@ -404,41 +447,25 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="18"/>
+    <n v="23"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="18"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <n v="18"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <n v="24"/>
-  </r>
-  <r>
-    <x v="18"/>
+    <n v="23"/>
+  </r>
+  <r>
+    <x v="21"/>
     <n v="24"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:F26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:F27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="22">
+      <items count="23">
         <item x="9"/>
         <item x="15"/>
         <item x="12"/>
@@ -450,6 +477,7 @@
         <item x="10"/>
         <item x="19"/>
         <item x="20"/>
+        <item x="21"/>
         <item x="8"/>
         <item x="5"/>
         <item x="1"/>
@@ -468,7 +496,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="22">
+  <rowItems count="23">
     <i>
       <x/>
     </i>
@@ -531,6 +559,9 @@
     </i>
     <i>
       <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
     </i>
     <i t="grand">
       <x/>
@@ -898,9 +929,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B54"/>
     </sheetView>
   </sheetViews>
@@ -923,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -931,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -955,7 +986,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -963,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -971,7 +1002,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -979,7 +1010,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1035,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1043,7 +1074,7 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1051,7 +1082,7 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1059,7 +1090,7 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1067,7 +1098,7 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1075,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1083,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1091,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1099,7 +1130,7 @@
         <v>12</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1115,7 +1146,7 @@
         <v>3</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1123,7 +1154,7 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1131,7 +1162,7 @@
         <v>13</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1179,7 +1210,7 @@
         <v>16</v>
       </c>
       <c r="B34">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1187,7 +1218,7 @@
         <v>17</v>
       </c>
       <c r="B35">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1195,7 +1226,7 @@
         <v>18</v>
       </c>
       <c r="B36">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1219,7 +1250,7 @@
         <v>16</v>
       </c>
       <c r="B39">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1227,7 +1258,7 @@
         <v>17</v>
       </c>
       <c r="B40">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1235,7 +1266,7 @@
         <v>32</v>
       </c>
       <c r="B41">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1259,7 +1290,7 @@
         <v>16</v>
       </c>
       <c r="B44">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1267,6 +1298,14 @@
         <v>17</v>
       </c>
       <c r="B45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46">
         <v>24</v>
       </c>
     </row>
@@ -1282,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1296,520 +1335,509 @@
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6">
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="5">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5">
-        <v>3</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="5">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5">
-        <v>4</v>
-      </c>
-      <c r="D10" s="5">
-        <v>4</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5">
-        <v>22</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5">
-        <v>4</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="5">
-        <v>29</v>
-      </c>
-      <c r="C14" s="5">
-        <v>29</v>
-      </c>
-      <c r="D14" s="5">
-        <v>29</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="5">
-        <v>18</v>
-      </c>
-      <c r="C15" s="5">
-        <v>18</v>
-      </c>
-      <c r="D15" s="5">
-        <v>18</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="5">
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C16" s="5">
-        <v>4</v>
-      </c>
-      <c r="D16" s="5">
-        <v>3</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0.47140452079103168</v>
-      </c>
-      <c r="F16" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="5">
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C17" s="5">
-        <v>4</v>
-      </c>
-      <c r="D17" s="5">
-        <v>3</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0.47140452079103168</v>
-      </c>
-      <c r="F17" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5">
-        <v>10</v>
-      </c>
-      <c r="C18" s="5">
-        <v>22</v>
-      </c>
-      <c r="D18" s="5">
-        <v>4</v>
-      </c>
-      <c r="E18" s="5">
-        <v>8.4852813742385695</v>
-      </c>
-      <c r="F18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="5">
-        <v>23.333333333333332</v>
-      </c>
-      <c r="C19" s="5">
-        <v>28</v>
-      </c>
-      <c r="D19" s="5">
-        <v>18</v>
-      </c>
-      <c r="E19" s="5">
-        <v>4.1096093353126513</v>
-      </c>
-      <c r="F19" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="5">
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C20" s="5">
-        <v>4</v>
-      </c>
-      <c r="D20" s="5">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0.47140452079103168</v>
-      </c>
-      <c r="F20" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="5">
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C21" s="5">
-        <v>4</v>
-      </c>
-      <c r="D21" s="5">
-        <v>3</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0.47140452079103168</v>
-      </c>
-      <c r="F21" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="5">
-        <v>23.333333333333332</v>
-      </c>
-      <c r="C22" s="5">
-        <v>28</v>
-      </c>
-      <c r="D22" s="5">
-        <v>18</v>
-      </c>
-      <c r="E22" s="5">
-        <v>4.1096093353126513</v>
-      </c>
-      <c r="F22" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="5">
-        <v>10</v>
-      </c>
-      <c r="C23" s="5">
-        <v>22</v>
-      </c>
-      <c r="D23" s="5">
-        <v>4</v>
-      </c>
-      <c r="E23" s="5">
-        <v>8.4852813742385695</v>
-      </c>
-      <c r="F23" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="5">
-        <v>7.7045454545454541</v>
-      </c>
-      <c r="C26" s="5">
-        <v>29</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
-        <v>9.1566655936202253</v>
-      </c>
-      <c r="F26" s="5">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
     <row r="1" spans="1:7" ht="25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4">
+        <v>20</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="4">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.81649658092772603</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.47140452079103168</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4">
+        <v>10.333333333333334</v>
+      </c>
+      <c r="C19" s="4">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4</v>
+      </c>
+      <c r="E19" s="4">
+        <v>7.5865377844940278</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4">
+        <v>19</v>
+      </c>
+      <c r="E20" s="4">
+        <v>4.5460605656619517</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.94280904158206336</v>
+      </c>
+      <c r="F21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.47140452079103168</v>
+      </c>
+      <c r="F22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4">
+        <v>23.666666666666668</v>
+      </c>
+      <c r="C23" s="4">
+        <v>29</v>
+      </c>
+      <c r="D23" s="4">
+        <v>19</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4.1096093353126513</v>
+      </c>
+      <c r="F23" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4">
+        <v>10.333333333333334</v>
+      </c>
+      <c r="C24" s="4">
+        <v>21</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4</v>
+      </c>
+      <c r="E24" s="4">
+        <v>7.5865377844940278</v>
+      </c>
+      <c r="F24" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4">
+        <v>8.844444444444445</v>
+      </c>
+      <c r="C27" s="4">
+        <v>31</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>9.3046118924507439</v>
+      </c>
+      <c r="F27" s="4">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This fixes #113, fixes #109,fixes #107, fixes #102, and fixes #96
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -11,11 +11,11 @@
     <sheet name="Pivot" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$46</definedName>
+    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$52</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
   <si>
     <t>mlclient::internals::AuthenticatingProxy::putSync</t>
   </si>
@@ -232,9 +232,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42502.3341349537" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="45">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42510.791856944445" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="51">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:B46" sheet="Linked Data From CSV"/>
+    <worksheetSource ref="A1:B52" sheet="Linked Data From CSV"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Function name" numFmtId="0">
@@ -264,7 +264,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="28"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="35"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -276,14 +276,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="45">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="51">
   <r>
     <x v="0"/>
-    <n v="8"/>
+    <n v="9"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="8"/>
+    <n v="9"/>
   </r>
   <r>
     <x v="2"/>
@@ -294,6 +294,54 @@
     <n v="0"/>
   </r>
   <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="4"/>
     <n v="4"/>
   </r>
@@ -302,8 +350,8 @@
     <n v="4"/>
   </r>
   <r>
-    <x v="6"/>
-    <n v="4"/>
+    <x v="11"/>
+    <n v="5"/>
   </r>
   <r>
     <x v="7"/>
@@ -314,88 +362,52 @@
     <n v="3"/>
   </r>
   <r>
-    <x v="9"/>
+    <x v="12"/>
     <n v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="6"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="6"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <n v="7"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="3"/>
     <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <n v="4"/>
-  </r>
-  <r>
     <x v="3"/>
     <n v="0"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="14"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="7"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="8"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="15"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="16"/>
@@ -406,16 +418,20 @@
     <n v="0"/>
   </r>
   <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="17"/>
-    <n v="26"/>
+    <n v="33"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="27"/>
+    <n v="33"/>
   </r>
   <r>
     <x v="19"/>
-    <n v="28"/>
+    <n v="35"/>
   </r>
   <r>
     <x v="16"/>
@@ -426,16 +442,20 @@
     <n v="0"/>
   </r>
   <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="17"/>
-    <n v="18"/>
+    <n v="19"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="18"/>
+    <n v="19"/>
   </r>
   <r>
     <x v="20"/>
-    <n v="19"/>
+    <n v="20"/>
   </r>
   <r>
     <x v="16"/>
@@ -446,22 +466,26 @@
     <n v="0"/>
   </r>
   <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="17"/>
-    <n v="25"/>
+    <n v="29"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="25"/>
+    <n v="29"/>
   </r>
   <r>
     <x v="21"/>
-    <n v="27"/>
+    <n v="31"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:F27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -929,9 +953,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B54"/>
     </sheetView>
   </sheetViews>
@@ -954,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -962,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -983,31 +1007,31 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1015,7 +1039,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1023,7 +1047,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1031,79 +1055,79 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1111,7 +1135,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1119,7 +1143,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1127,7 +1151,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1135,103 +1159,103 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B34">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B36">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1239,39 +1263,39 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B39">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B40">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B41">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1290,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="B44">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1298,15 +1322,63 @@
         <v>17</v>
       </c>
       <c r="B45">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>33</v>
       </c>
-      <c r="B46">
-        <v>27</v>
+      <c r="B52">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1405,13 +1477,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -1445,13 +1517,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -1465,13 +1537,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -1485,13 +1557,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -1545,13 +1617,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -1565,13 +1637,13 @@
         <v>18</v>
       </c>
       <c r="B14" s="4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C14" s="4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D14" s="4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -1585,13 +1657,13 @@
         <v>32</v>
       </c>
       <c r="B15" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -1605,13 +1677,13 @@
         <v>33</v>
       </c>
       <c r="B16" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -1625,16 +1697,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="4">
-        <v>3</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="C17" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
       </c>
       <c r="E17" s="4">
-        <v>0</v>
+        <v>0.47140452079103168</v>
       </c>
       <c r="F17" s="4">
         <v>3</v>
@@ -1645,7 +1717,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="4">
-        <v>3.3333333333333335</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
@@ -1665,16 +1737,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4">
-        <v>5.666666666666667</v>
+        <v>6</v>
       </c>
       <c r="C19" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" s="4">
-        <v>2.0548046676563256</v>
+        <v>2.1602468994692869</v>
       </c>
       <c r="F19" s="4">
         <v>3</v>
@@ -1685,16 +1757,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="4">
-        <v>23.333333333333332</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D20" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="4">
-        <v>3.858612300930075</v>
+        <v>5.8878405775518976</v>
       </c>
       <c r="F20" s="4">
         <v>3</v>
@@ -1705,16 +1777,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="4">
-        <v>3</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="C21" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
       <c r="E21" s="4">
-        <v>0</v>
+        <v>0.47140452079103168</v>
       </c>
       <c r="F21" s="4">
         <v>3</v>
@@ -1725,7 +1797,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="4">
-        <v>3.3333333333333335</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="C22" s="4">
         <v>4</v>
@@ -1745,16 +1817,16 @@
         <v>16</v>
       </c>
       <c r="B23" s="4">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C23" s="4">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D23" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E23" s="4">
-        <v>3.5590260840104371</v>
+        <v>5.8878405775518976</v>
       </c>
       <c r="F23" s="4">
         <v>3</v>
@@ -1765,16 +1837,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="4">
-        <v>5.666666666666667</v>
+        <v>6</v>
       </c>
       <c r="C24" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" s="4">
-        <v>2.0548046676563256</v>
+        <v>2.1602468994692869</v>
       </c>
       <c r="F24" s="4">
         <v>3</v>
@@ -1797,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1825,19 +1897,19 @@
         <v>20</v>
       </c>
       <c r="B27" s="4">
-        <v>7.2</v>
+        <v>7.1764705882352944</v>
       </c>
       <c r="C27" s="4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
       </c>
       <c r="E27" s="4">
-        <v>8.6810137656842823</v>
+        <v>10.04051768517888</v>
       </c>
       <c r="F27" s="4">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top level search result info support. Re-run of performance stats
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17300" tabRatio="500" activeTab="1"/>
@@ -11,7 +11,7 @@
     <sheet name="Pivot" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$52</definedName>
+    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$59</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
   <si>
     <t>mlclient::internals::AuthenticatingProxy::putSync</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>ConnectionSearchTest::testWordQuery</t>
+  </si>
+  <si>
+    <t>mlclient::utilities::CppRestJsonHelper::fromResponse</t>
+  </si>
+  <si>
+    <t>SearchResultSetTest::testEmptySearch</t>
   </si>
 </sst>
 </file>
@@ -232,13 +238,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42510.791856944445" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="51">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42517.022459490741" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="58">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:B52" sheet="Linked Data From CSV"/>
+    <worksheetSource ref="A1:B59" sheet="Linked Data From CSV"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Function name" numFmtId="0">
-      <sharedItems count="22">
+      <sharedItems count="24">
         <s v="mlclient::internals::AuthenticatingProxy::putSync"/>
         <s v="mlclient::Connection::saveDocument"/>
         <s v="ConnectionDocumentCrudTest::testSaveJson"/>
@@ -261,10 +267,12 @@
         <s v="ConnectionSearchTest::testEmptySearch"/>
         <s v="ConnectionSearchTest::testQueryText"/>
         <s v="ConnectionSearchTest::testWordQuery"/>
+        <s v="mlclient::utilities::CppRestJsonHelper::fromResponse"/>
+        <s v="SearchResultSetTest::testEmptySearch"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="35"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="34"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -276,18 +284,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="51">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="58">
   <r>
     <x v="0"/>
-    <n v="9"/>
+    <n v="14"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="9"/>
+    <n v="15"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="9"/>
+    <n v="15"/>
   </r>
   <r>
     <x v="3"/>
@@ -299,15 +307,15 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="6"/>
-    <n v="3"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="7"/>
@@ -323,6 +331,50 @@
   </r>
   <r>
     <x v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
     <n v="5"/>
   </r>
   <r>
@@ -330,8 +382,8 @@
     <n v="5"/>
   </r>
   <r>
-    <x v="10"/>
-    <n v="5"/>
+    <x v="13"/>
+    <n v="6"/>
   </r>
   <r>
     <x v="3"/>
@@ -350,8 +402,8 @@
     <n v="4"/>
   </r>
   <r>
-    <x v="11"/>
-    <n v="5"/>
+    <x v="14"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="7"/>
@@ -362,20 +414,12 @@
     <n v="3"/>
   </r>
   <r>
-    <x v="12"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="15"/>
     <n v="4"/>
   </r>
   <r>
-    <x v="1"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <n v="4"/>
+    <x v="16"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -386,28 +430,16 @@
     <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <n v="4"/>
+    <x v="17"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="30"/>
   </r>
   <r>
     <x v="16"/>
@@ -423,15 +455,15 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="33"/>
+    <n v="22"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="33"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <n v="35"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="23"/>
   </r>
   <r>
     <x v="16"/>
@@ -447,15 +479,15 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="19"/>
+    <n v="32"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="19"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <n v="20"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="34"/>
   </r>
   <r>
     <x v="16"/>
@@ -471,25 +503,29 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="29"/>
+    <n v="21"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="29"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <n v="31"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="24"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:F27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:F29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="23">
+      <items count="25">
         <item x="9"/>
         <item x="15"/>
         <item x="12"/>
@@ -512,6 +548,8 @@
         <item x="0"/>
         <item x="3"/>
         <item x="16"/>
+        <item x="22"/>
+        <item x="23"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -520,7 +558,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="23">
+  <rowItems count="25">
     <i>
       <x/>
     </i>
@@ -586,6 +624,12 @@
     </i>
     <i>
       <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
     </i>
     <i t="grand">
       <x/>
@@ -953,15 +997,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B72" sqref="A2:B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -978,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -986,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -994,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1018,7 +1062,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1026,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1034,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1066,7 +1110,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1074,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1082,7 +1126,7 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1122,7 +1166,7 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1154,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1162,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1170,7 +1214,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1218,7 +1262,7 @@
         <v>6</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1226,7 +1270,7 @@
         <v>7</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1266,7 +1310,7 @@
         <v>16</v>
       </c>
       <c r="B38">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1274,7 +1318,7 @@
         <v>17</v>
       </c>
       <c r="B39">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1282,7 +1326,7 @@
         <v>18</v>
       </c>
       <c r="B40">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1314,7 +1358,7 @@
         <v>16</v>
       </c>
       <c r="B44">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1322,7 +1366,7 @@
         <v>17</v>
       </c>
       <c r="B45">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1330,7 +1374,7 @@
         <v>32</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1362,7 +1406,7 @@
         <v>16</v>
       </c>
       <c r="B50">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1370,7 +1414,7 @@
         <v>17</v>
       </c>
       <c r="B51">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1378,7 +1422,63 @@
         <v>33</v>
       </c>
       <c r="B52">
-        <v>31</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1493,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
@@ -1401,7 +1501,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -1517,13 +1617,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -1557,13 +1657,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -1577,13 +1677,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -1597,13 +1697,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -1617,13 +1717,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -1637,13 +1737,13 @@
         <v>18</v>
       </c>
       <c r="B14" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -1657,13 +1757,13 @@
         <v>32</v>
       </c>
       <c r="B15" s="4">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -1677,13 +1777,13 @@
         <v>33</v>
       </c>
       <c r="B16" s="4">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D16" s="4">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -1697,16 +1797,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="4">
-        <v>3.3333333333333335</v>
+        <v>3</v>
       </c>
       <c r="C17" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
       </c>
       <c r="E17" s="4">
-        <v>0.47140452079103168</v>
+        <v>0</v>
       </c>
       <c r="F17" s="4">
         <v>3</v>
@@ -1717,16 +1817,16 @@
         <v>4</v>
       </c>
       <c r="B18" s="4">
-        <v>3.6666666666666665</v>
+        <v>4</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
       </c>
       <c r="D18" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="4">
-        <v>0.47140452079103168</v>
+        <v>0</v>
       </c>
       <c r="F18" s="4">
         <v>3</v>
@@ -1737,16 +1837,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D19" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4">
-        <v>2.1602468994692869</v>
+        <v>4.3204937989385739</v>
       </c>
       <c r="F19" s="4">
         <v>3</v>
@@ -1757,19 +1857,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="4">
-        <v>27</v>
+        <v>26.25</v>
       </c>
       <c r="C20" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="4">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E20" s="4">
-        <v>5.8878405775518976</v>
+        <v>4.3803538669838078</v>
       </c>
       <c r="F20" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1777,16 +1877,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="4">
-        <v>3.3333333333333335</v>
+        <v>3</v>
       </c>
       <c r="C21" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
       <c r="E21" s="4">
-        <v>0.47140452079103168</v>
+        <v>0</v>
       </c>
       <c r="F21" s="4">
         <v>3</v>
@@ -1797,16 +1897,16 @@
         <v>3</v>
       </c>
       <c r="B22" s="4">
-        <v>3.6666666666666665</v>
+        <v>4</v>
       </c>
       <c r="C22" s="4">
         <v>4</v>
       </c>
       <c r="D22" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="4">
-        <v>0.47140452079103168</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <v>3</v>
@@ -1817,19 +1917,19 @@
         <v>16</v>
       </c>
       <c r="B23" s="4">
-        <v>27</v>
+        <v>25.75</v>
       </c>
       <c r="C23" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E23" s="4">
-        <v>5.8878405775518976</v>
+        <v>4.4930501889028571</v>
       </c>
       <c r="F23" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1837,16 +1937,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="4">
-        <v>6</v>
+        <v>8.6666666666666661</v>
       </c>
       <c r="C24" s="4">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D24" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" s="4">
-        <v>2.1602468994692869</v>
+        <v>3.858612300930075</v>
       </c>
       <c r="F24" s="4">
         <v>3</v>
@@ -1869,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1889,27 +1989,67 @@
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="4">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4">
+        <v>24</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="4">
-        <v>7.1764705882352944</v>
-      </c>
-      <c r="C27" s="4">
-        <v>35</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
-        <v>10.04051768517888</v>
-      </c>
-      <c r="F27" s="4">
-        <v>51</v>
+      <c r="B29" s="4">
+        <v>8</v>
+      </c>
+      <c r="C29" s="4">
+        <v>34</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>10.277192693297739</v>
+      </c>
+      <c r="F29" s="4">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completion of Collections listing. Fixes #158
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Pivot" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$59</definedName>
+    <definedName name="performance" localSheetId="0">'Linked Data From CSV'!$A$2:$B$64</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
   <si>
     <t>mlclient::internals::AuthenticatingProxy::putSync</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>SearchResultSetTest::testEmptySearch</t>
+  </si>
+  <si>
+    <t>ConnectionCollectionsTest::testListTopLevelCollections</t>
   </si>
 </sst>
 </file>
@@ -238,13 +241,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42517.022459490741" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="58">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Fowler" refreshedDate="42529.688381712964" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="63">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:B59" sheet="Linked Data From CSV"/>
+    <worksheetSource ref="A1:B64" sheet="Linked Data From CSV"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Function name" numFmtId="0">
-      <sharedItems count="24">
+      <sharedItems count="25">
         <s v="mlclient::internals::AuthenticatingProxy::putSync"/>
         <s v="mlclient::Connection::saveDocument"/>
         <s v="ConnectionDocumentCrudTest::testSaveJson"/>
@@ -269,10 +272,11 @@
         <s v="ConnectionSearchTest::testWordQuery"/>
         <s v="mlclient::utilities::CppRestJsonHelper::fromResponse"/>
         <s v="SearchResultSetTest::testEmptySearch"/>
+        <s v="ConnectionCollectionsTest::testListTopLevelCollections"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="34"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="31"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -284,18 +288,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="58">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="63">
   <r>
     <x v="0"/>
-    <n v="14"/>
+    <n v="16"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="15"/>
+    <n v="16"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="15"/>
+    <n v="17"/>
   </r>
   <r>
     <x v="3"/>
@@ -307,15 +311,59 @@
   </r>
   <r>
     <x v="4"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
     <n v="4"/>
   </r>
   <r>
+    <x v="8"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="7"/>
+  </r>
+  <r>
     <x v="5"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="4"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="7"/>
   </r>
   <r>
     <x v="7"/>
@@ -326,20 +374,20 @@
     <n v="3"/>
   </r>
   <r>
-    <x v="9"/>
+    <x v="12"/>
     <n v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="7"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="7"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <n v="7"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="4"/>
   </r>
   <r>
     <x v="3"/>
@@ -351,39 +399,31 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="4"/>
+    <n v="3"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <n v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3"/>
   </r>
   <r>
     <x v="7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="15"/>
     <n v="3"/>
   </r>
   <r>
-    <x v="8"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="5"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="5"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <n v="6"/>
+    <x v="16"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -394,28 +434,16 @@
     <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <n v="4"/>
+    <x v="17"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="31"/>
   </r>
   <r>
     <x v="16"/>
@@ -431,15 +459,15 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="28"/>
+    <n v="21"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="29"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <n v="30"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="22"/>
   </r>
   <r>
     <x v="16"/>
@@ -455,15 +483,15 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="22"/>
+    <n v="26"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="22"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <n v="23"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="28"/>
   </r>
   <r>
     <x v="16"/>
@@ -479,19 +507,19 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="32"/>
+    <n v="24"/>
   </r>
   <r>
     <x v="18"/>
-    <n v="32"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <n v="34"/>
-  </r>
-  <r>
-    <x v="16"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="22"/>
     <n v="0"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="26"/>
   </r>
   <r>
     <x v="3"/>
@@ -503,29 +531,26 @@
   </r>
   <r>
     <x v="17"/>
-    <n v="21"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <n v="22"/>
+    <n v="13"/>
   </r>
   <r>
     <x v="22"/>
     <n v="0"/>
   </r>
   <r>
-    <x v="23"/>
-    <n v="24"/>
+    <x v="24"/>
+    <n v="14"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:F29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:F30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="25">
+      <items count="26">
+        <item x="24"/>
         <item x="9"/>
         <item x="15"/>
         <item x="12"/>
@@ -558,7 +583,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="25">
+  <rowItems count="26">
     <i>
       <x/>
     </i>
@@ -630,6 +655,9 @@
     </i>
     <i>
       <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
     </i>
     <i t="grand">
       <x/>
@@ -997,15 +1025,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B72" sqref="A2:B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1022,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1030,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1038,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1062,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1070,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1078,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1086,7 +1114,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1094,7 +1122,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1102,7 +1130,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1110,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1118,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1126,7 +1154,7 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1150,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1158,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1166,7 +1194,7 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1198,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1206,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1214,7 +1242,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1238,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1246,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1254,7 +1282,7 @@
         <v>13</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1262,7 +1290,7 @@
         <v>6</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1270,7 +1298,7 @@
         <v>7</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1278,7 +1306,7 @@
         <v>14</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1310,7 +1338,7 @@
         <v>16</v>
       </c>
       <c r="B38">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1318,7 +1346,7 @@
         <v>17</v>
       </c>
       <c r="B39">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1326,7 +1354,7 @@
         <v>18</v>
       </c>
       <c r="B40">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1358,7 +1386,7 @@
         <v>16</v>
       </c>
       <c r="B44">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1366,7 +1394,7 @@
         <v>17</v>
       </c>
       <c r="B45">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1374,7 +1402,7 @@
         <v>32</v>
       </c>
       <c r="B46">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1406,7 +1434,7 @@
         <v>16</v>
       </c>
       <c r="B50">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1414,7 +1442,7 @@
         <v>17</v>
       </c>
       <c r="B51">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1422,7 +1450,7 @@
         <v>33</v>
       </c>
       <c r="B52">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1454,7 +1482,7 @@
         <v>16</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1462,7 +1490,7 @@
         <v>17</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1478,7 +1506,47 @@
         <v>35</v>
       </c>
       <c r="B59">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1493,7 +1561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
@@ -1501,7 +1569,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -1554,16 +1622,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -1574,7 +1642,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -1594,7 +1662,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1614,16 +1682,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -1634,16 +1702,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -1654,16 +1722,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -1674,16 +1742,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -1694,16 +1762,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B12" s="4">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -1714,16 +1782,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -1734,16 +1802,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D14" s="4">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -1754,16 +1822,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -1774,16 +1842,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -1794,39 +1862,39 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D17" s="4">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E17" s="4">
         <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
       </c>
       <c r="D18" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18" s="4">
-        <v>0</v>
+        <v>0.81649658092772603</v>
       </c>
       <c r="F18" s="4">
         <v>3</v>
@@ -1834,19 +1902,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="4">
-        <v>9</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="C19" s="4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D19" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="4">
-        <v>4.3204937989385739</v>
+        <v>1.699673171197595</v>
       </c>
       <c r="F19" s="4">
         <v>3</v>
@@ -1854,59 +1922,59 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B20" s="4">
-        <v>26.25</v>
+        <v>8.6666666666666661</v>
       </c>
       <c r="C20" s="4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D20" s="4">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E20" s="4">
-        <v>4.3803538669838078</v>
+        <v>5.2493385826745405</v>
       </c>
       <c r="F20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4">
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="C21" s="4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D21" s="4">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E21" s="4">
-        <v>0</v>
+        <v>3.3541019662496847</v>
       </c>
       <c r="F21" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B22" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="4">
         <v>4</v>
       </c>
       <c r="D22" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22" s="4">
-        <v>0</v>
+        <v>0.81649658092772603</v>
       </c>
       <c r="F22" s="4">
         <v>3</v>
@@ -1914,67 +1982,67 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B23" s="4">
-        <v>25.75</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="C23" s="4">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D23" s="4">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E23" s="4">
-        <v>4.4930501889028571</v>
+        <v>1.699673171197595</v>
       </c>
       <c r="F23" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B24" s="4">
-        <v>8.6666666666666661</v>
+        <v>22.6</v>
       </c>
       <c r="C24" s="4">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D24" s="4">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4">
+        <v>5.4626001134990654</v>
+      </c>
+      <c r="F24" s="4">
         <v>5</v>
-      </c>
-      <c r="E24" s="4">
-        <v>3.858612300930075</v>
-      </c>
-      <c r="F24" s="4">
-        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B25" s="4">
-        <v>0</v>
+        <v>8.6666666666666661</v>
       </c>
       <c r="C25" s="4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D25" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25" s="4">
-        <v>0</v>
+        <v>5.2493385826745405</v>
       </c>
       <c r="F25" s="4">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4">
         <v>0</v>
@@ -1989,12 +2057,12 @@
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B27" s="4">
         <v>0</v>
@@ -2009,47 +2077,67 @@
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C28" s="4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E28" s="4">
         <v>0</v>
       </c>
       <c r="F28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="4">
+        <v>26</v>
+      </c>
+      <c r="C29" s="4">
+        <v>26</v>
+      </c>
+      <c r="D29" s="4">
+        <v>26</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="4">
-        <v>8</v>
-      </c>
-      <c r="C29" s="4">
-        <v>34</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="4">
-        <v>10.277192693297739</v>
-      </c>
-      <c r="F29" s="4">
-        <v>58</v>
+      <c r="B30" s="4">
+        <v>7.7936507936507935</v>
+      </c>
+      <c r="C30" s="4">
+        <v>31</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>9.72177841552638</v>
+      </c>
+      <c r="F30" s="4">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>